<commit_message>
Made ControlPlantState obsolete and merged control plant logic with experimental plant logic
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Control</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>lost a leaf when scanning</t>
+  </si>
+  <si>
+    <t>Leaves on tip little wrinkly</t>
+  </si>
+  <si>
+    <t>Leaves on tip more wrinkly</t>
   </si>
 </sst>
 </file>
@@ -71,10 +77,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -378,24 +384,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
         <v>41727</v>
       </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="2"/>
+      <c r="D1" s="1">
+        <v>41728</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -406,26 +417,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -435,16 +455,28 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -453,8 +485,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Experimentation changeover command and plant data
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,9 +396,13 @@
     <col min="5" max="5" width="24.140625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>41727</v>
       </c>
@@ -411,8 +415,20 @@
         <v>41729</v>
       </c>
       <c r="G1" s="2"/>
+      <c r="H1" s="1">
+        <v>41730</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="1">
+        <v>41731</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="1">
+        <v>41732</v>
+      </c>
+      <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -423,7 +439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -439,8 +455,17 @@
       <c r="F3">
         <v>18</v>
       </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>21</v>
+      </c>
+      <c r="L3">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -456,8 +481,17 @@
       <c r="F4">
         <v>12</v>
       </c>
+      <c r="H4">
+        <v>13</v>
+      </c>
+      <c r="J4">
+        <v>13</v>
+      </c>
+      <c r="L4">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -476,8 +510,17 @@
       <c r="F5">
         <v>10</v>
       </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="L5">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -493,23 +536,47 @@
       <c r="F6">
         <v>21</v>
       </c>
+      <c r="H6">
+        <v>22</v>
+      </c>
+      <c r="J6">
+        <v>22</v>
+      </c>
+      <c r="L6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7">
         <v>11</v>
       </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
       <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+      <c r="L7">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New images and log updates
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Control</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Leaves on tip more wrinkly</t>
+  </si>
+  <si>
+    <t>Leaves becoming spotty</t>
+  </si>
+  <si>
+    <t>Tip leaves feel dry</t>
   </si>
 </sst>
 </file>
@@ -384,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,9 +406,14 @@
     <col min="10" max="10" width="9.42578125" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>41727</v>
       </c>
@@ -427,8 +438,24 @@
         <v>41732</v>
       </c>
       <c r="M1" s="2"/>
+      <c r="N1" s="1">
+        <v>41733</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="1">
+        <v>41734</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="1">
+        <v>41735</v>
+      </c>
+      <c r="S1" s="2"/>
+      <c r="T1" s="1">
+        <v>41736</v>
+      </c>
+      <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -438,8 +465,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -464,8 +494,20 @@
       <c r="L3">
         <v>21</v>
       </c>
+      <c r="N3">
+        <v>21</v>
+      </c>
+      <c r="P3">
+        <v>21</v>
+      </c>
+      <c r="R3">
+        <v>21</v>
+      </c>
+      <c r="T3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -490,8 +532,20 @@
       <c r="L4">
         <v>13</v>
       </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="P4">
+        <v>13</v>
+      </c>
+      <c r="R4">
+        <v>13</v>
+      </c>
+      <c r="T4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -519,8 +573,20 @@
       <c r="L5">
         <v>11</v>
       </c>
+      <c r="N5">
+        <v>11</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -545,8 +611,17 @@
       <c r="L6">
         <v>22</v>
       </c>
+      <c r="N6">
+        <v>22</v>
+      </c>
+      <c r="P6">
+        <v>23</v>
+      </c>
+      <c r="R6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -568,10 +643,23 @@
       <c r="L7">
         <v>11</v>
       </c>
+      <c r="N7">
+        <v>11</v>
+      </c>
+      <c r="P7">
+        <v>12</v>
+      </c>
+      <c r="R7">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>

</xml_diff>

<commit_message>
Leaf data and prepare database commands for new experiment
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="15315" windowHeight="5700"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="15315" windowHeight="5640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Control</t>
   </si>
@@ -46,6 +46,36 @@
   </si>
   <si>
     <t>Tip leaves feel dry</t>
+  </si>
+  <si>
+    <t>Lost a leaf at the tip. Tip dry</t>
+  </si>
+  <si>
+    <t>Tip brown</t>
+  </si>
+  <si>
+    <t>Bottom brown</t>
+  </si>
+  <si>
+    <t>Leaf</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>0.0019370</t>
+  </si>
+  <si>
+    <t>0.0019703</t>
+  </si>
+  <si>
+    <t>0.0019559</t>
+  </si>
+  <si>
+    <t>0.0019708</t>
+  </si>
+  <si>
+    <t>0.0018701</t>
   </si>
 </sst>
 </file>
@@ -61,17 +91,96 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -81,14 +190,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:BR7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM3" sqref="AM3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,250 +560,775 @@
     <col min="17" max="17" width="20.7109375" customWidth="1"/>
     <col min="19" max="19" width="16.140625" customWidth="1"/>
     <col min="21" max="21" width="15.5703125" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="26" max="26" width="9" customWidth="1"/>
+    <col min="27" max="27" width="27.85546875" customWidth="1"/>
+    <col min="29" max="29" width="20.28515625" customWidth="1"/>
+    <col min="31" max="31" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="1">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
         <v>41727</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1">
+      <c r="C1" s="3"/>
+      <c r="D1" s="2">
         <v>41728</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="1">
+      <c r="E1" s="3"/>
+      <c r="F1" s="2">
         <v>41729</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1">
+      <c r="G1" s="3"/>
+      <c r="H1" s="2">
         <v>41730</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="1">
+      <c r="I1" s="3"/>
+      <c r="J1" s="2">
         <v>41731</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="1">
+      <c r="K1" s="3"/>
+      <c r="L1" s="2">
         <v>41732</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1">
+      <c r="M1" s="3"/>
+      <c r="N1" s="2">
         <v>41733</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="1">
+      <c r="O1" s="3"/>
+      <c r="P1" s="2">
         <v>41734</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="1">
+      <c r="Q1" s="3"/>
+      <c r="R1" s="2">
         <v>41735</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="1">
+      <c r="S1" s="3"/>
+      <c r="T1" s="2">
         <v>41736</v>
       </c>
-      <c r="U1" s="2"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="2">
+        <v>41737</v>
+      </c>
+      <c r="W1" s="3"/>
+      <c r="X1" s="2">
+        <v>41738</v>
+      </c>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="2">
+        <v>41739</v>
+      </c>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="2">
+        <v>41742</v>
+      </c>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="4">
+        <v>41743</v>
+      </c>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="9">
+        <v>41744</v>
+      </c>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="15"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="13"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="15"/>
+      <c r="BG1" s="10"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="13"/>
+      <c r="BK1" s="14"/>
+      <c r="BL1" s="15"/>
+      <c r="BM1" s="10"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="16"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="6"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="6"/>
+      <c r="AV2" s="6"/>
+      <c r="AW2" s="6"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="6"/>
+      <c r="BB2" s="6"/>
+      <c r="BC2" s="6"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="6"/>
+      <c r="BH2" s="6"/>
+      <c r="BI2" s="6"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="6"/>
+      <c r="BN2" s="6"/>
+      <c r="BO2" s="6"/>
+      <c r="BP2" s="6"/>
+      <c r="BQ2" s="6"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>18</v>
       </c>
-      <c r="F3">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
         <v>18</v>
       </c>
-      <c r="H3">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
         <v>20</v>
       </c>
-      <c r="J3">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1">
         <v>21</v>
       </c>
-      <c r="L3">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1">
         <v>21</v>
       </c>
-      <c r="N3">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1">
         <v>21</v>
       </c>
-      <c r="P3">
+      <c r="O3" s="1"/>
+      <c r="P3" s="1">
         <v>21</v>
       </c>
-      <c r="R3">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1">
         <v>21</v>
       </c>
-      <c r="T3">
+      <c r="S3" s="1"/>
+      <c r="T3" s="1">
         <v>22</v>
       </c>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1">
+        <v>22</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="6">
+        <v>34</v>
+      </c>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="8">
+        <v>36</v>
+      </c>
+      <c r="AG3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
+      <c r="AQ3" s="6"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="6"/>
+      <c r="AV3" s="6"/>
+      <c r="AW3" s="6"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="6"/>
+      <c r="BB3" s="6"/>
+      <c r="BC3" s="6"/>
+      <c r="BD3" s="8"/>
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="8"/>
+      <c r="BG3" s="6"/>
+      <c r="BH3" s="6"/>
+      <c r="BI3" s="6"/>
+      <c r="BJ3" s="8"/>
+      <c r="BK3" s="8"/>
+      <c r="BL3" s="8"/>
+      <c r="BM3" s="6"/>
+      <c r="BN3" s="6"/>
+      <c r="BO3" s="6"/>
+      <c r="BP3" s="6"/>
+      <c r="BQ3" s="6"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>11</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="1">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>12</v>
       </c>
-      <c r="H4">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
         <v>13</v>
       </c>
-      <c r="J4">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
         <v>13</v>
       </c>
-      <c r="L4">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1">
         <v>13</v>
       </c>
-      <c r="N4">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
         <v>13</v>
       </c>
-      <c r="P4">
+      <c r="O4" s="1"/>
+      <c r="P4" s="1">
         <v>13</v>
       </c>
-      <c r="R4">
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1">
         <v>13</v>
       </c>
-      <c r="T4">
+      <c r="S4" s="1"/>
+      <c r="T4" s="1">
         <v>14</v>
       </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1">
+        <v>14</v>
+      </c>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1">
+        <v>15</v>
+      </c>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="6">
+        <v>18</v>
+      </c>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="8">
+        <v>18</v>
+      </c>
+      <c r="AG4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="6"/>
+      <c r="AV4" s="6"/>
+      <c r="AW4" s="6"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="6"/>
+      <c r="BB4" s="6"/>
+      <c r="BC4" s="6"/>
+      <c r="BD4" s="8"/>
+      <c r="BE4" s="8"/>
+      <c r="BF4" s="8"/>
+      <c r="BG4" s="6"/>
+      <c r="BH4" s="6"/>
+      <c r="BI4" s="6"/>
+      <c r="BJ4" s="8"/>
+      <c r="BK4" s="8"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="6"/>
+      <c r="BN4" s="6"/>
+      <c r="BO4" s="6"/>
+      <c r="BP4" s="6"/>
+      <c r="BQ4" s="6"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
         <v>10</v>
       </c>
-      <c r="J5">
-        <v>11</v>
-      </c>
-      <c r="L5">
-        <v>11</v>
-      </c>
-      <c r="N5">
-        <v>11</v>
-      </c>
-      <c r="P5">
-        <v>11</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1">
+        <v>11</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1">
+        <v>11</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1">
+        <v>11</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R5">
-        <v>11</v>
-      </c>
+      <c r="R5" s="1">
+        <v>11</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1">
+        <v>11</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1">
+        <v>11</v>
+      </c>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1">
+        <v>12</v>
+      </c>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1">
+        <v>12</v>
+      </c>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="6">
+        <v>12</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF5" s="8">
+        <v>12</v>
+      </c>
+      <c r="AG5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="8"/>
+      <c r="AS5" s="8"/>
+      <c r="AT5" s="8"/>
+      <c r="AU5" s="6"/>
+      <c r="AV5" s="6"/>
+      <c r="AW5" s="6"/>
+      <c r="AX5" s="8"/>
+      <c r="AY5" s="8"/>
+      <c r="AZ5" s="8"/>
+      <c r="BA5" s="6"/>
+      <c r="BB5" s="6"/>
+      <c r="BC5" s="6"/>
+      <c r="BD5" s="8"/>
+      <c r="BE5" s="8"/>
+      <c r="BF5" s="8"/>
+      <c r="BG5" s="6"/>
+      <c r="BH5" s="6"/>
+      <c r="BI5" s="6"/>
+      <c r="BJ5" s="8"/>
+      <c r="BK5" s="8"/>
+      <c r="BL5" s="8"/>
+      <c r="BM5" s="6"/>
+      <c r="BN5" s="6"/>
+      <c r="BO5" s="6"/>
+      <c r="BP5" s="6"/>
+      <c r="BQ5" s="6"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>21</v>
       </c>
-      <c r="H6">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
         <v>22</v>
       </c>
-      <c r="J6">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
         <v>22</v>
       </c>
-      <c r="L6">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
         <v>22</v>
       </c>
-      <c r="N6">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
         <v>22</v>
       </c>
-      <c r="P6">
+      <c r="O6" s="1"/>
+      <c r="P6" s="1">
         <v>23</v>
       </c>
-      <c r="R6">
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1">
         <v>24</v>
       </c>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1">
+        <v>24</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1">
+        <v>25</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1">
+        <v>27</v>
+      </c>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1">
+        <v>26</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>29</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD6" s="6">
+        <v>28</v>
+      </c>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="8">
+        <v>27</v>
+      </c>
+      <c r="AG6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="6"/>
+      <c r="AR6" s="8"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="6"/>
+      <c r="AV6" s="6"/>
+      <c r="AW6" s="6"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+      <c r="BA6" s="6"/>
+      <c r="BB6" s="6"/>
+      <c r="BC6" s="6"/>
+      <c r="BD6" s="8"/>
+      <c r="BE6" s="8"/>
+      <c r="BF6" s="8"/>
+      <c r="BG6" s="6"/>
+      <c r="BH6" s="6"/>
+      <c r="BI6" s="6"/>
+      <c r="BJ6" s="8"/>
+      <c r="BK6" s="8"/>
+      <c r="BL6" s="8"/>
+      <c r="BM6" s="6"/>
+      <c r="BN6" s="6"/>
+      <c r="BO6" s="6"/>
+      <c r="BP6" s="6"/>
+      <c r="BQ6" s="6"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
-      <c r="F7">
-        <v>11</v>
-      </c>
-      <c r="H7">
-        <v>11</v>
-      </c>
-      <c r="J7">
-        <v>11</v>
-      </c>
-      <c r="L7">
-        <v>11</v>
-      </c>
-      <c r="N7">
-        <v>11</v>
-      </c>
-      <c r="P7">
+      <c r="B7" s="1">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
+        <v>11</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
+        <v>11</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1">
         <v>12</v>
       </c>
-      <c r="R7">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1">
         <v>12</v>
       </c>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1">
+        <v>12</v>
+      </c>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1">
+        <v>12</v>
+      </c>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1">
+        <v>12</v>
+      </c>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1">
+        <v>12</v>
+      </c>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="6">
+        <v>13</v>
+      </c>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="8">
+        <v>14</v>
+      </c>
+      <c r="AG7" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="8"/>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="8"/>
+      <c r="AS7" s="8"/>
+      <c r="AT7" s="8"/>
+      <c r="AU7" s="6"/>
+      <c r="AV7" s="6"/>
+      <c r="AW7" s="6"/>
+      <c r="AX7" s="8"/>
+      <c r="AY7" s="8"/>
+      <c r="AZ7" s="8"/>
+      <c r="BA7" s="6"/>
+      <c r="BB7" s="6"/>
+      <c r="BC7" s="6"/>
+      <c r="BD7" s="8"/>
+      <c r="BE7" s="8"/>
+      <c r="BF7" s="8"/>
+      <c r="BG7" s="6"/>
+      <c r="BH7" s="6"/>
+      <c r="BI7" s="6"/>
+      <c r="BJ7" s="8"/>
+      <c r="BK7" s="8"/>
+      <c r="BL7" s="8"/>
+      <c r="BM7" s="6"/>
+      <c r="BN7" s="6"/>
+      <c r="BO7" s="6"/>
+      <c r="BP7" s="6"/>
+      <c r="BQ7" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="28">
+    <mergeCell ref="BJ1:BL1"/>
+    <mergeCell ref="BM1:BO1"/>
+    <mergeCell ref="BP1:BR1"/>
+    <mergeCell ref="AU1:AW1"/>
+    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="BA1:BC1"/>
+    <mergeCell ref="BD1:BF1"/>
+    <mergeCell ref="BG1:BI1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AR1:AT1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>

</xml_diff>